<commit_message>
feat: comparison and results
</commit_message>
<xml_diff>
--- a/Results/results.xlsx
+++ b/Results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcoturetta/Projects/trees/Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6EDFAB52-20CF-D243-A3DD-7EAFFEB24834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CBC83D-D2FF-4649-A29F-BDC922967343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-2640" windowWidth="38400" windowHeight="21600" activeTab="5" xr2:uid="{C2DFFE4D-25A2-1745-B2DF-3A724F43E27B}"/>
   </bookViews>
@@ -17,16 +17,17 @@
     <sheet name="second_attempt" sheetId="2" r:id="rId2"/>
     <sheet name="third_attempt" sheetId="3" r:id="rId3"/>
     <sheet name="fourth_attempt" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet6" sheetId="7" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">first_attempt!$D$1:$D$22</definedName>
+    <definedName name="Flow_merged_1" localSheetId="5">Sheet1!$A$2:$N$31</definedName>
     <definedName name="FlowORT_all_merged_1" localSheetId="0">first_attempt!$A$2:$L$21</definedName>
     <definedName name="FlowORT_merged_v2" localSheetId="1">second_attempt!$A$2:$O$21</definedName>
     <definedName name="FlowORT_merged_v3" localSheetId="2">third_attempt!$A$2:$T$21</definedName>
     <definedName name="FlowORT_merged_v4" localSheetId="3">fourth_attempt!$A$2:$AL$21</definedName>
-    <definedName name="FlowORT_merged_v4" localSheetId="5">Sheet5!$A$2:$S$21</definedName>
+    <definedName name="FlowORT_merged_v4" localSheetId="4">Sheet5!$A$2:$S$21</definedName>
     <definedName name="FlowORT_merged_v4_1" localSheetId="3">fourth_attempt!$K$1:$AC$20</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
@@ -51,9 +52,11 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{E5B01EC0-85A1-694A-8A87-86CEB14F732F}" name="FlowORT_all_merged" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_all_merged.csv" tab="0" comma="1">
-      <textFields count="12">
+  <connection id="1" xr16:uid="{0B7E41EF-F552-0546-8AD2-56F2646A41D4}" name="Flow_merged" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/Flow_merged.csv" tab="0" comma="1">
+      <textFields count="14">
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
         <textField/>
@@ -69,13 +72,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{941BD38D-E8AD-1247-82C7-BEF5727070FD}" name="FlowORT_merged_v2" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v2.csv" tab="0" comma="1">
-      <textFields count="16">
-        <textField/>
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="2" xr16:uid="{E5B01EC0-85A1-694A-8A87-86CEB14F732F}" name="FlowORT_all_merged" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_all_merged.csv" tab="0" comma="1">
+      <textFields count="12">
         <textField/>
         <textField/>
         <textField/>
@@ -91,12 +90,9 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{0EBA7137-B2C9-2144-978E-C9D085068167}" name="FlowORT_merged_v3" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v3.csv" tab="0" comma="1">
-      <textFields count="19">
-        <textField/>
-        <textField/>
-        <textField/>
+  <connection id="3" xr16:uid="{941BD38D-E8AD-1247-82C7-BEF5727070FD}" name="FlowORT_merged_v2" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v2.csv" tab="0" comma="1">
+      <textFields count="16">
         <textField/>
         <textField/>
         <textField/>
@@ -116,8 +112,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{8D29B154-FBD1-DC4A-9265-E6B4451FA048}" name="FlowORT_merged_v4" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v4.csv" tab="0" comma="1">
+  <connection id="4" xr16:uid="{0EBA7137-B2C9-2144-978E-C9D085068167}" name="FlowORT_merged_v3" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v3.csv" tab="0" comma="1">
       <textFields count="19">
         <textField/>
         <textField/>
@@ -141,8 +137,8 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" xr16:uid="{9161CE35-2BAA-5844-8FC7-A53E04DF7D87}" name="FlowORT_merged_v41" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v4.csv" tab="0" comma="1">
+  <connection id="5" xr16:uid="{8D29B154-FBD1-DC4A-9265-E6B4451FA048}" name="FlowORT_merged_v4" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v4.csv" tab="0" comma="1">
       <textFields count="19">
         <textField/>
         <textField/>
@@ -166,8 +162,33 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{1A684BC6-0443-C543-B065-88FA3DDEEE34}" name="FlowORT_merged_v42" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v4.csv" tab="0" comma="1">
+  <connection id="6" xr16:uid="{9161CE35-2BAA-5844-8FC7-A53E04DF7D87}" name="FlowORT_merged_v41" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v4.csv" tab="0" comma="1">
+      <textFields count="19">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" xr16:uid="{1A684BC6-0443-C543-B065-88FA3DDEEE34}" name="FlowORT_merged_v42" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/marcoturetta/Projects/trees/Results/FlowORT_merged_v4.csv" tab="0" comma="1">
       <textFields count="19">
         <textField/>
         <textField/>
@@ -195,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="29">
   <si>
     <t>balance-scale_enc.csv</t>
   </si>
@@ -280,6 +301,9 @@
   <si>
     <t>bnf_differring</t>
   </si>
+  <si>
+    <t>FlowOCT</t>
+  </si>
 </sst>
 </file>
 
@@ -336,27 +360,31 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_all_merged_1" connectionId="1" xr16:uid="{1AD55309-0D61-8E48-85C2-0F9C6D35A546}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_all_merged_1" connectionId="2" xr16:uid="{1AD55309-0D61-8E48-85C2-0F9C6D35A546}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v2" connectionId="2" xr16:uid="{AB427A97-A8CA-1C4B-A483-2FC0FBD21A59}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v2" connectionId="3" xr16:uid="{AB427A97-A8CA-1C4B-A483-2FC0FBD21A59}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v3" connectionId="3" xr16:uid="{8ED1988E-0927-5E46-8704-AAC51168F2F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v3" connectionId="4" xr16:uid="{8ED1988E-0927-5E46-8704-AAC51168F2F3}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v4_1" connectionId="5" xr16:uid="{5724890A-2D58-8745-9BF2-6D1057180765}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v4" connectionId="5" xr16:uid="{52677210-1B18-234D-BF83-FD4B2CB96AE0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v4" connectionId="4" xr16:uid="{52677210-1B18-234D-BF83-FD4B2CB96AE0}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v4_1" connectionId="6" xr16:uid="{5724890A-2D58-8745-9BF2-6D1057180765}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v4" connectionId="6" xr16:uid="{C13CF44E-4974-A746-AFD5-CAD319201F09}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="FlowORT_merged_v4" connectionId="7" xr16:uid="{C13CF44E-4974-A746-AFD5-CAD319201F09}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Flow_merged_1" connectionId="1" xr16:uid="{98192304-7506-2C45-B7AD-62A6B0EA9245}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6160,23 +6188,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{725AFF7F-D598-D144-A1A5-17E5B891E655}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{462351F1-8094-EB44-85A8-8AB28DF3869E}">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7445,4 +7461,1401 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C53E818-756D-B44F-AF99-655B8DC88A51}">
+  <dimension ref="A1:N31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>625</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>3600</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>-864</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>121</v>
+      </c>
+      <c r="J2">
+        <v>4.4468698501586896</v>
+      </c>
+      <c r="K2">
+        <v>-4.8630393996246903</v>
+      </c>
+      <c r="L2">
+        <v>2.3039999999999998</v>
+      </c>
+      <c r="M2">
+        <v>1.3824000000000001</v>
+      </c>
+      <c r="N2">
+        <v>-1.5637982195845599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>625</v>
+      </c>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>3600</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>5213</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1798</v>
+      </c>
+      <c r="J3">
+        <v>74.126079082488999</v>
+      </c>
+      <c r="K3">
+        <v>1.87552115905773E-2</v>
+      </c>
+      <c r="L3">
+        <v>0.3856</v>
+      </c>
+      <c r="M3">
+        <v>0.34079999999999999</v>
+      </c>
+      <c r="N3">
+        <v>0.36795252225519198</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>625</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>3600</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>213</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>11491</v>
+      </c>
+      <c r="J4">
+        <v>235.17185783386199</v>
+      </c>
+      <c r="K4">
+        <v>1.87552115905773E-2</v>
+      </c>
+      <c r="L4">
+        <v>0.3856</v>
+      </c>
+      <c r="M4">
+        <v>0.34079999999999999</v>
+      </c>
+      <c r="N4">
+        <v>0.36795252225519198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>277</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>3600</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>-62</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>7544</v>
+      </c>
+      <c r="J5">
+        <v>24.701692819595301</v>
+      </c>
+      <c r="K5">
+        <v>-8.1758629377677694E-2</v>
+      </c>
+      <c r="L5">
+        <v>0.223826714801444</v>
+      </c>
+      <c r="M5">
+        <v>0.223826714801444</v>
+      </c>
+      <c r="N5">
+        <v>0.234567901234567</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>277</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>3600</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>1169.99999999999</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>5620</v>
+      </c>
+      <c r="J6">
+        <v>33.745861291885298</v>
+      </c>
+      <c r="K6">
+        <v>-8.1758629377676806E-2</v>
+      </c>
+      <c r="L6">
+        <v>0.223826714801444</v>
+      </c>
+      <c r="M6">
+        <v>0.223826714801444</v>
+      </c>
+      <c r="N6">
+        <v>0.234567901234567</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>277</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>3600</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>62</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>11684</v>
+      </c>
+      <c r="J7">
+        <v>114.32020306587199</v>
+      </c>
+      <c r="K7">
+        <v>-8.1758629377676806E-2</v>
+      </c>
+      <c r="L7">
+        <v>0.223826714801444</v>
+      </c>
+      <c r="M7">
+        <v>0.223826714801444</v>
+      </c>
+      <c r="N7">
+        <v>0.234567901234567</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>132</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>3600</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>-111</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>61</v>
+      </c>
+      <c r="J8">
+        <v>0.267576694488525</v>
+      </c>
+      <c r="K8">
+        <v>-1.2019315188762001</v>
+      </c>
+      <c r="L8">
+        <v>1.2954545454545401</v>
+      </c>
+      <c r="M8">
+        <v>0.84090909090909005</v>
+      </c>
+      <c r="N8">
+        <v>-0.37037037037037002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>132</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>3600</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>1110.99999999999</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>2133</v>
+      </c>
+      <c r="J9">
+        <v>2.7174580097198402</v>
+      </c>
+      <c r="K9">
+        <v>0.21451565700907199</v>
+      </c>
+      <c r="L9">
+        <v>0.46212121212121199</v>
+      </c>
+      <c r="M9">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="N9">
+        <v>0.32098765432098703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10">
+        <v>132</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>3600</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>54.999996000000003</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>2520</v>
+      </c>
+      <c r="J10">
+        <v>5.05781698226928</v>
+      </c>
+      <c r="K10">
+        <v>0.21451565700907199</v>
+      </c>
+      <c r="L10">
+        <v>0.46212121212121199</v>
+      </c>
+      <c r="M10">
+        <v>0.41666666666666602</v>
+      </c>
+      <c r="N10">
+        <v>0.32098765432098703</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11">
+        <v>232</v>
+      </c>
+      <c r="D11">
+        <v>2</v>
+      </c>
+      <c r="E11">
+        <v>3600</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>-7</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>322</v>
+      </c>
+      <c r="J11">
+        <v>1.0001893043518</v>
+      </c>
+      <c r="K11">
+        <v>0.87873357228195803</v>
+      </c>
+      <c r="L11">
+        <v>3.0172413793103401E-2</v>
+      </c>
+      <c r="M11">
+        <v>3.0172413793103401E-2</v>
+      </c>
+      <c r="N11">
+        <v>0.93518518518518501</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>232</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3600</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <v>935</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>193</v>
+      </c>
+      <c r="J12">
+        <v>1.6961710453033401</v>
+      </c>
+      <c r="K12">
+        <v>0.87873357228195903</v>
+      </c>
+      <c r="L12">
+        <v>3.0172413793103401E-2</v>
+      </c>
+      <c r="M12">
+        <v>3.0172413793103401E-2</v>
+      </c>
+      <c r="N12">
+        <v>0.93518518518518501</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>232</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>3600</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13">
+        <v>7</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>789</v>
+      </c>
+      <c r="J13">
+        <v>5.1695299148559499</v>
+      </c>
+      <c r="K13">
+        <v>0.87873357228195903</v>
+      </c>
+      <c r="L13">
+        <v>3.0172413793103401E-2</v>
+      </c>
+      <c r="M13">
+        <v>3.0172413793103401E-2</v>
+      </c>
+      <c r="N13">
+        <v>0.93518518518518501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>267</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>3600</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>-55</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>9935</v>
+      </c>
+      <c r="J14">
+        <v>12.729445934295599</v>
+      </c>
+      <c r="K14">
+        <v>-0.259433962264149</v>
+      </c>
+      <c r="L14">
+        <v>0.205992509363295</v>
+      </c>
+      <c r="M14">
+        <v>0.205992509363295</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>267</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="E15">
+        <v>3600</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>1123</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>6497</v>
+      </c>
+      <c r="J15">
+        <v>16.496693849563599</v>
+      </c>
+      <c r="K15">
+        <v>-0.259433962264151</v>
+      </c>
+      <c r="L15">
+        <v>0.205992509363295</v>
+      </c>
+      <c r="M15">
+        <v>0.205992509363295</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>267</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="E16">
+        <v>3600</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="G16">
+        <v>54.999999672266597</v>
+      </c>
+      <c r="H16" s="2">
+        <v>5.0909224614273496E-9</v>
+      </c>
+      <c r="I16">
+        <v>10254</v>
+      </c>
+      <c r="J16">
+        <v>59.533364057540801</v>
+      </c>
+      <c r="K16">
+        <v>-0.259433962264151</v>
+      </c>
+      <c r="L16">
+        <v>0.205992509363295</v>
+      </c>
+      <c r="M16">
+        <v>0.205992509363295</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>625</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>3600</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>-864</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>20408</v>
+      </c>
+      <c r="J17">
+        <v>506.88257384300198</v>
+      </c>
+      <c r="K17">
+        <v>-4.8630393996246903</v>
+      </c>
+      <c r="L17">
+        <v>2.3039999999999998</v>
+      </c>
+      <c r="M17">
+        <v>1.3824000000000001</v>
+      </c>
+      <c r="N17">
+        <v>-1.5637982195845599</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>625</v>
+      </c>
+      <c r="D18">
+        <v>3</v>
+      </c>
+      <c r="E18">
+        <v>3600</v>
+      </c>
+      <c r="F18">
+        <v>9</v>
+      </c>
+      <c r="G18">
+        <v>15183.9999999999</v>
+      </c>
+      <c r="H18">
+        <v>8.5616438355876998E-2</v>
+      </c>
+      <c r="I18">
+        <v>198907</v>
+      </c>
+      <c r="J18">
+        <v>3600.7476761340999</v>
+      </c>
+      <c r="K18">
+        <v>7.9828538670024901E-2</v>
+      </c>
+      <c r="L18">
+        <v>0.36159999999999098</v>
+      </c>
+      <c r="M18">
+        <v>0.29440000000000799</v>
+      </c>
+      <c r="N18">
+        <v>0.45400593471808398</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>625</v>
+      </c>
+      <c r="D19">
+        <v>3</v>
+      </c>
+      <c r="E19">
+        <v>3600</v>
+      </c>
+      <c r="F19">
+        <v>9</v>
+      </c>
+      <c r="G19">
+        <v>191.99999852941099</v>
+      </c>
+      <c r="H19">
+        <v>100</v>
+      </c>
+      <c r="I19">
+        <v>19768</v>
+      </c>
+      <c r="J19">
+        <v>3600.6980011463102</v>
+      </c>
+      <c r="K19">
+        <v>1.4683656451949001E-2</v>
+      </c>
+      <c r="L19">
+        <v>0.38719999999999999</v>
+      </c>
+      <c r="M19">
+        <v>0.30719999999999997</v>
+      </c>
+      <c r="N19">
+        <v>0.43026706231453998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>277</v>
+      </c>
+      <c r="D20">
+        <v>3</v>
+      </c>
+      <c r="E20">
+        <v>3600</v>
+      </c>
+      <c r="F20">
+        <v>9</v>
+      </c>
+      <c r="G20">
+        <v>-54</v>
+      </c>
+      <c r="H20">
+        <v>72.222222222221902</v>
+      </c>
+      <c r="I20">
+        <v>801826</v>
+      </c>
+      <c r="J20">
+        <v>3601.2127518653801</v>
+      </c>
+      <c r="K20">
+        <v>5.7823129251699898E-2</v>
+      </c>
+      <c r="L20">
+        <v>0.19494584837545101</v>
+      </c>
+      <c r="M20">
+        <v>0.19494584837545101</v>
+      </c>
+      <c r="N20">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>277</v>
+      </c>
+      <c r="D21">
+        <v>3</v>
+      </c>
+      <c r="E21">
+        <v>3600</v>
+      </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>3378</v>
+      </c>
+      <c r="H21">
+        <v>1.1943087625814</v>
+      </c>
+      <c r="I21">
+        <v>351845</v>
+      </c>
+      <c r="J21">
+        <v>3600.4451830387102</v>
+      </c>
+      <c r="K21">
+        <v>5.7823129251700703E-2</v>
+      </c>
+      <c r="L21">
+        <v>0.19494584837545101</v>
+      </c>
+      <c r="M21">
+        <v>0.19494584837545101</v>
+      </c>
+      <c r="N21">
+        <v>0.33333333333333298</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>277</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>3600</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <v>54.999997944148703</v>
+      </c>
+      <c r="H22">
+        <v>100</v>
+      </c>
+      <c r="I22">
+        <v>42777</v>
+      </c>
+      <c r="J22">
+        <v>3600.4791548252101</v>
+      </c>
+      <c r="K22">
+        <v>4.0375409423028502E-2</v>
+      </c>
+      <c r="L22">
+        <v>0.19855595667869999</v>
+      </c>
+      <c r="M22">
+        <v>0.19855595667869999</v>
+      </c>
+      <c r="N22">
+        <v>0.32098765432098703</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>132</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+      <c r="E23">
+        <v>3600</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <v>-111</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+      <c r="I23">
+        <v>7269</v>
+      </c>
+      <c r="J23">
+        <v>3.7664110660552899</v>
+      </c>
+      <c r="K23">
+        <v>-1.2019315188762001</v>
+      </c>
+      <c r="L23">
+        <v>1.2954545454545401</v>
+      </c>
+      <c r="M23">
+        <v>0.84090909090909005</v>
+      </c>
+      <c r="N23">
+        <v>-0.37037037037037002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>132</v>
+      </c>
+      <c r="D24">
+        <v>3</v>
+      </c>
+      <c r="E24">
+        <v>3600</v>
+      </c>
+      <c r="F24">
+        <v>2</v>
+      </c>
+      <c r="G24">
+        <v>3206</v>
+      </c>
+      <c r="H24">
+        <v>8.3177375753577393E-3</v>
+      </c>
+      <c r="I24">
+        <v>61513</v>
+      </c>
+      <c r="J24">
+        <v>114.617954969406</v>
+      </c>
+      <c r="K24">
+        <v>0.43342112964588803</v>
+      </c>
+      <c r="L24">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="M24">
+        <v>0.28787878787878701</v>
+      </c>
+      <c r="N24">
+        <v>0.530864197530864</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>132</v>
+      </c>
+      <c r="D25">
+        <v>3</v>
+      </c>
+      <c r="E25">
+        <v>3600</v>
+      </c>
+      <c r="F25">
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <v>37.999998756056698</v>
+      </c>
+      <c r="H25">
+        <v>65.664159277006803</v>
+      </c>
+      <c r="I25">
+        <v>626725</v>
+      </c>
+      <c r="J25">
+        <v>3600.1148979663799</v>
+      </c>
+      <c r="K25">
+        <v>0.45917474510702599</v>
+      </c>
+      <c r="L25">
+        <v>0.31818180027019499</v>
+      </c>
+      <c r="M25">
+        <v>0.28787879683459999</v>
+      </c>
+      <c r="N25">
+        <v>0.53086418293620596</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26">
+        <v>232</v>
+      </c>
+      <c r="D26">
+        <v>3</v>
+      </c>
+      <c r="E26">
+        <v>3600</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>-5</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>186445</v>
+      </c>
+      <c r="J26">
+        <v>354.60639691352799</v>
+      </c>
+      <c r="K26">
+        <v>0.91338112305854202</v>
+      </c>
+      <c r="L26">
+        <v>2.1551724137931001E-2</v>
+      </c>
+      <c r="M26">
+        <v>2.1551724137931001E-2</v>
+      </c>
+      <c r="N26">
+        <v>0.95370370370370305</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>12</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27">
+        <v>232</v>
+      </c>
+      <c r="D27">
+        <v>3</v>
+      </c>
+      <c r="E27">
+        <v>3600</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27">
+        <v>2785</v>
+      </c>
+      <c r="H27">
+        <v>9.79272074436849E-3</v>
+      </c>
+      <c r="I27">
+        <v>13386</v>
+      </c>
+      <c r="J27">
+        <v>155.03478193282999</v>
+      </c>
+      <c r="K27">
+        <v>-0.64575866188769304</v>
+      </c>
+      <c r="L27">
+        <v>0.409482758620689</v>
+      </c>
+      <c r="M27">
+        <v>0.409482758620689</v>
+      </c>
+      <c r="N27">
+        <v>0.12037037037037</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>232</v>
+      </c>
+      <c r="D28">
+        <v>3</v>
+      </c>
+      <c r="E28">
+        <v>3600</v>
+      </c>
+      <c r="F28">
+        <v>9</v>
+      </c>
+      <c r="G28">
+        <v>4.9999976753816604</v>
+      </c>
+      <c r="H28">
+        <v>100</v>
+      </c>
+      <c r="I28">
+        <v>76925</v>
+      </c>
+      <c r="J28">
+        <v>3600.2755441665599</v>
+      </c>
+      <c r="K28">
+        <v>0.91338112305854202</v>
+      </c>
+      <c r="L28">
+        <v>2.1551724137931001E-2</v>
+      </c>
+      <c r="M28">
+        <v>2.1551724137931001E-2</v>
+      </c>
+      <c r="N28">
+        <v>0.95370370370370305</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>267</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>3600</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29">
+        <v>-48</v>
+      </c>
+      <c r="H29">
+        <v>9.8502758076139205E-3</v>
+      </c>
+      <c r="I29">
+        <v>334698</v>
+      </c>
+      <c r="J29">
+        <v>3373.2225041389402</v>
+      </c>
+      <c r="K29">
+        <v>-9.9142367066894194E-2</v>
+      </c>
+      <c r="L29">
+        <v>0.17977528089887601</v>
+      </c>
+      <c r="M29">
+        <v>0.17977528089887601</v>
+      </c>
+      <c r="N29">
+        <v>0.12727272727272701</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>12</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30">
+        <v>267</v>
+      </c>
+      <c r="D30">
+        <v>3</v>
+      </c>
+      <c r="E30">
+        <v>3600</v>
+      </c>
+      <c r="F30">
+        <v>9</v>
+      </c>
+      <c r="G30">
+        <v>3252</v>
+      </c>
+      <c r="H30">
+        <v>4.6125461254444701E-2</v>
+      </c>
+      <c r="I30">
+        <v>749717</v>
+      </c>
+      <c r="J30">
+        <v>3600.3199172019899</v>
+      </c>
+      <c r="K30">
+        <v>-9.9142367066895304E-2</v>
+      </c>
+      <c r="L30">
+        <v>0.17977528089887601</v>
+      </c>
+      <c r="M30">
+        <v>0.17977528089887601</v>
+      </c>
+      <c r="N30">
+        <v>0.12727272727272701</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>13</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31">
+        <v>267</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>3600</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <v>48</v>
+      </c>
+      <c r="H31">
+        <v>31.871880981678899</v>
+      </c>
+      <c r="I31">
+        <v>47814</v>
+      </c>
+      <c r="J31">
+        <v>3600.4014861583701</v>
+      </c>
+      <c r="K31">
+        <v>-9.9142367066895304E-2</v>
+      </c>
+      <c r="L31">
+        <v>0.17977528089887601</v>
+      </c>
+      <c r="M31">
+        <v>0.17977528089887601</v>
+      </c>
+      <c r="N31">
+        <v>0.12727272727272701</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S31">
+    <sortCondition ref="D2:D31"/>
+    <sortCondition ref="B2:B31"/>
+    <sortCondition ref="A2:A31"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>